<commit_message>
Some better resource management
</commit_message>
<xml_diff>
--- a/ResourceProbabilityWorksheet.xlsx
+++ b/ResourceProbabilityWorksheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>A</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Level 3 Mining Bot</t>
+  </si>
+  <si>
+    <t>Oxygen Producing Unit</t>
   </si>
 </sst>
 </file>
@@ -142,11 +145,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,38 +453,38 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
@@ -501,7 +504,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
@@ -524,7 +527,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
@@ -547,7 +550,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
@@ -570,7 +573,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
@@ -593,7 +596,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
@@ -616,38 +619,38 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12">
@@ -670,7 +673,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>2</v>
       </c>
       <c r="B13">
@@ -693,7 +696,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>3</v>
       </c>
       <c r="B14">
@@ -716,7 +719,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>4</v>
       </c>
       <c r="B15">
@@ -739,7 +742,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>5</v>
       </c>
       <c r="B16">
@@ -762,7 +765,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>6</v>
       </c>
       <c r="B17">
@@ -785,38 +788,38 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21">
@@ -839,7 +842,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>2</v>
       </c>
       <c r="B22">
@@ -862,7 +865,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>3</v>
       </c>
       <c r="B23">
@@ -885,7 +888,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>4</v>
       </c>
       <c r="B24">
@@ -908,7 +911,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>5</v>
       </c>
       <c r="B25">
@@ -931,7 +934,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>6</v>
       </c>
       <c r="B26">
@@ -954,38 +957,38 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="B29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>1</v>
       </c>
       <c r="B30">
@@ -1008,7 +1011,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>2</v>
       </c>
       <c r="B31">
@@ -1031,7 +1034,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>3</v>
       </c>
       <c r="B32">
@@ -1054,7 +1057,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>4</v>
       </c>
       <c r="B33">
@@ -1077,7 +1080,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>5</v>
       </c>
       <c r="B34">
@@ -1100,7 +1103,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>6</v>
       </c>
       <c r="B35">
@@ -1123,38 +1126,38 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="A37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="B38" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>1</v>
       </c>
       <c r="B39">
@@ -1177,7 +1180,7 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>2</v>
       </c>
       <c r="B40">
@@ -1200,7 +1203,7 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>3</v>
       </c>
       <c r="B41">
@@ -1223,7 +1226,7 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>4</v>
       </c>
       <c r="B42">
@@ -1246,7 +1249,7 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>5</v>
       </c>
       <c r="B43">
@@ -1269,7 +1272,7 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>6</v>
       </c>
       <c r="B44">
@@ -1292,38 +1295,38 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="B47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="B47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>1</v>
       </c>
       <c r="B48">
@@ -1346,7 +1349,7 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>2</v>
       </c>
       <c r="B49">
@@ -1369,7 +1372,7 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>3</v>
       </c>
       <c r="B50">
@@ -1392,7 +1395,7 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>4</v>
       </c>
       <c r="B51">
@@ -1415,7 +1418,7 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>5</v>
       </c>
       <c r="B52">
@@ -1438,7 +1441,7 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>6</v>
       </c>
       <c r="B53">
@@ -1462,12 +1465,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A46:G46"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A46:G46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1475,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1493,7 +1496,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -1528,194 +1531,211 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>5</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>25</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="B11" t="s">
-        <v>23</v>
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>50</v>
-      </c>
-      <c r="F13">
-        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
-        <f>CEILING(B13*1.5,1)</f>
+      <c r="B15">
+        <f>CEILING(B14*1.5,1)</f>
         <v>38</v>
       </c>
-      <c r="C14">
-        <f t="shared" ref="C14:F14" si="0">CEILING(C13*1.5,1)</f>
+      <c r="C15">
+        <f t="shared" ref="C15:F15" si="0">CEILING(C14*1.5,1)</f>
         <v>15</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B15">
-        <f>CEILING(B14*1.5,1)</f>
+      <c r="B16">
+        <f>CEILING(B15*1.5,1)</f>
         <v>57</v>
       </c>
-      <c r="C15">
-        <f t="shared" ref="C15" si="1">CEILING(C14*1.5,1)</f>
+      <c r="C16">
+        <f t="shared" ref="C16" si="1">CEILING(C15*1.5,1)</f>
         <v>23</v>
       </c>
-      <c r="D15">
-        <f t="shared" ref="D15" si="2">CEILING(D14*1.5,1)</f>
+      <c r="D16">
+        <f t="shared" ref="D16" si="2">CEILING(D15*1.5,1)</f>
         <v>12</v>
       </c>
-      <c r="E15">
-        <f t="shared" ref="E15" si="3">CEILING(E14*1.5,1)</f>
+      <c r="E16">
+        <f t="shared" ref="E16" si="3">CEILING(E15*1.5,1)</f>
         <v>113</v>
       </c>
-      <c r="F15">
-        <f t="shared" ref="F15" si="4">CEILING(F14*1.5,1)</f>
+      <c r="F16">
+        <f t="shared" ref="F16" si="4">CEILING(F15*1.5,1)</f>
         <v>1125</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The word bot has no meaning anymore.
</commit_message>
<xml_diff>
--- a/ResourceProbabilityWorksheet.xlsx
+++ b/ResourceProbabilityWorksheet.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1481,7 +1481,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Set up a tutorial point.
</commit_message>
<xml_diff>
--- a/ResourceProbabilityWorksheet.xlsx
+++ b/ResourceProbabilityWorksheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>A</t>
   </si>
@@ -100,13 +100,16 @@
   </si>
   <si>
     <t>Oxygen Producing Unit</t>
+  </si>
+  <si>
+    <t>Not implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +121,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,13 +153,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,15 +464,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="1" t="s">
@@ -619,15 +630,15 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" s="1" t="s">
@@ -788,15 +799,15 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" s="1" t="s">
@@ -957,15 +968,15 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="1" t="s">
@@ -1126,15 +1137,15 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
+      <c r="A37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7">
       <c r="B38" s="1" t="s">
@@ -1295,15 +1306,15 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" s="1" t="s">
@@ -1478,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1490,12 +1501,12 @@
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1512,41 +1523,44 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" s="3" customFormat="1">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>25</v>
       </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="3" customFormat="1">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="B4" s="3">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1563,34 +1577,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>300</v>
       </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="B7" s="3">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1607,7 +1633,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1624,7 +1650,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1641,12 +1667,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="B12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -1663,7 +1689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1683,59 +1709,59 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <f>CEILING(B14*1.5,1)</f>
         <v>38</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <f t="shared" ref="C15:F15" si="0">CEILING(C14*1.5,1)</f>
         <v>15</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
+    <row r="16" spans="1:8">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <f>CEILING(B15*1.5,1)</f>
         <v>57</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <f t="shared" ref="C16" si="1">CEILING(C15*1.5,1)</f>
         <v>23</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <f t="shared" ref="D16" si="2">CEILING(D15*1.5,1)</f>
         <v>12</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <f t="shared" ref="E16" si="3">CEILING(E15*1.5,1)</f>
         <v>113</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <f t="shared" ref="F16" si="4">CEILING(F15*1.5,1)</f>
         <v>1125</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Artifact handler should work.
</commit_message>
<xml_diff>
--- a/ResourceProbabilityWorksheet.xlsx
+++ b/ResourceProbabilityWorksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="30">
   <si>
     <t>A</t>
   </si>
@@ -103,13 +103,16 @@
   </si>
   <si>
     <t>Not implemented</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +131,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,14 +164,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,26 +467,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7">
+    <row r="1" spans="1:16">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,153 +506,260 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:16">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C7">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,117 +778,159 @@
       <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F12">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1">
         <v>2</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D13">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F13">
         <v>50</v>
       </c>
       <c r="G13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1">
         <v>3</v>
       </c>
       <c r="B14">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1">
         <v>4</v>
       </c>
       <c r="B15">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D15">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F15">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:16">
       <c r="A16" s="1">
         <v>5</v>
       </c>
       <c r="B16">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C16">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D16">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F16">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -780,7 +941,7 @@
         <v>6</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>40</v>
@@ -789,25 +950,25 @@
         <v>40</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" s="1" t="s">
@@ -846,7 +1007,7 @@
         <v>10</v>
       </c>
       <c r="F21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G21">
         <v>10</v>
@@ -860,19 +1021,19 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D22">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E22">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="F22">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -880,22 +1041,22 @@
         <v>3</v>
       </c>
       <c r="B23">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D23">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -903,22 +1064,22 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -929,19 +1090,19 @@
         <v>20</v>
       </c>
       <c r="C25">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D25">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -949,34 +1110,34 @@
         <v>6</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D26">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="A28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="1" t="s">
@@ -1003,22 +1164,22 @@
         <v>1</v>
       </c>
       <c r="B30">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E30">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="G30">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1026,22 +1187,22 @@
         <v>2</v>
       </c>
       <c r="B31">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C31">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F31">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G31">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1049,22 +1210,22 @@
         <v>3</v>
       </c>
       <c r="B32">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C32">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F32">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="G32">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1072,22 +1233,22 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F33">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G33">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1095,22 +1256,22 @@
         <v>5</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C34">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F34">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G34">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1118,34 +1279,34 @@
         <v>6</v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C35">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F35">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G35">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="A37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7">
       <c r="B38" s="1" t="s">
@@ -1172,22 +1333,22 @@
         <v>1</v>
       </c>
       <c r="B39">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C39">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D39">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E39">
         <v>60</v>
       </c>
       <c r="F39">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G39">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1195,22 +1356,22 @@
         <v>2</v>
       </c>
       <c r="B40">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C40">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D40">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E40">
         <v>60</v>
       </c>
       <c r="F40">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G40">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1218,22 +1379,22 @@
         <v>3</v>
       </c>
       <c r="B41">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C41">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D41">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E41">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F41">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G41">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1241,22 +1402,22 @@
         <v>4</v>
       </c>
       <c r="B42">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C42">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D42">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E42">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="F42">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G42">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1264,22 +1425,22 @@
         <v>5</v>
       </c>
       <c r="B43">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C43">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D43">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E43">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="F43">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G43">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1287,34 +1448,34 @@
         <v>6</v>
       </c>
       <c r="B44">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C44">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D44">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E44">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="F44">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G44">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="A46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" s="1" t="s">
@@ -1341,22 +1502,19 @@
         <v>1</v>
       </c>
       <c r="B48">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>60</v>
-      </c>
-      <c r="F48">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1364,22 +1522,22 @@
         <v>2</v>
       </c>
       <c r="B49">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E49">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G49">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1387,22 +1545,22 @@
         <v>3</v>
       </c>
       <c r="B50">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1410,22 +1568,22 @@
         <v>4</v>
       </c>
       <c r="B51">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C51">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G51">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1433,22 +1591,22 @@
         <v>5</v>
       </c>
       <c r="B52">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C52">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D52">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1456,19 +1614,19 @@
         <v>6</v>
       </c>
       <c r="B53">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C53">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G53">
         <v>100</v>
@@ -1476,12 +1634,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A37:G37"/>
     <mergeCell ref="A46:G46"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A37:G37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1491,7 +1649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1523,40 +1681,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8" s="2" customFormat="1">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>25</v>
       </c>
-      <c r="C3" s="3">
-        <v>20</v>
-      </c>
-      <c r="D3" s="3">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:8" s="2" customFormat="1">
+      <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="3">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1578,36 +1736,36 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>300</v>
       </c>
-      <c r="C6" s="3">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="C6" s="2">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>25</v>
       </c>
-      <c r="C7" s="3">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1710,58 +1868,58 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <f>CEILING(B14*1.5,1)</f>
         <v>38</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <f t="shared" ref="C15:F15" si="0">CEILING(C14*1.5,1)</f>
         <v>15</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <f>CEILING(B15*1.5,1)</f>
         <v>57</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <f t="shared" ref="C16" si="1">CEILING(C15*1.5,1)</f>
         <v>23</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <f t="shared" ref="D16" si="2">CEILING(D15*1.5,1)</f>
         <v>12</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f t="shared" ref="E16" si="3">CEILING(E15*1.5,1)</f>
         <v>113</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <f t="shared" ref="F16" si="4">CEILING(F15*1.5,1)</f>
         <v>1125</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>